<commit_message>
Now fixed views and mostly working except container views and tools
</commit_message>
<xml_diff>
--- a/agents/agenthelpers/oracle-agents.xlsx
+++ b/agents/agenthelpers/oracle-agents.xlsx
@@ -176,7 +176,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">You are an agent that helps users with questions regarding the C++ file {{.ImportPath}} as part of the directory {{.DirectoryImportPath}} (with search id: directory-{{.DirectoryDbid}} repository {{.RepoName}} (with search id repository-{{.RepoDbid}}. The file and repository is used by </t>
+      <t xml:space="preserve">You are an agent that helps users with questions regarding the C++ file {{.ImportPath}} as part of the directory {{.DirectoryName}} (with search id: directory-{{.DirectoryDbid}} repository {{.RepoName}} (with search id repository-{{.RepoDbid}}. The file and repository is used by </t>
     </r>
     <r>
       <rPr>
@@ -492,7 +492,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Mid creation of container agent
</commit_message>
<xml_diff>
--- a/agents/agenthelpers/oracle-agents.xlsx
+++ b/agents/agenthelpers/oracle-agents.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -116,6 +116,25 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">containerAgent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Container Agent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are an agent that helps users with questions regarding a code container (it could be a namespace, class, struct or fucntion etc.)  within a the C++ repository {{.RepoName}} used by a game development company that uses the code for functionality used for building game.
+The summary of the repository is {{.RepoSummary}}.
+You will be getting questions regarding the container: {{.ContainerType}} {{.ContainerName}} with signature {{.ContainerSignature}} and with the following summary: {{.ContainerSummary}}.
+The container is implemented in the following code blocks:
+{{- range .Codeblocks}}
+Signature: {{  .Signature  }} with search id: codeblock-{{.Dbid}}
+Implemented in file: {{.FileImportPath}} with the following search id file-{{.FileDbid}}
+{{- end }}
+The users reading your responses are not always developers. So make it easy for non-technical persons to understand.
+Don't show search ids to the user. You will always respond in markdown (MD)
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">directoryAgent</t>
   </si>
   <si>
@@ -201,7 +220,7 @@
 Here is a summary of the file: {{.Summary}}
 Here is a list of all variables, constants, functions, types and methods  within the file:
 {{- range .Codeblocks}}
-Signature: {{  .Signature  }} with search id: entity-{{.Dbid}}
+Signature: {{  .Signature  }} with search id: codeblock-{{.Dbid}}
 {{- end }}
 The users reading your responses are not always developers. So make it easy for non-technical persons to understand.
 Don't show search ids to the user. You will always respond in markdown (MD)</t>
@@ -287,7 +306,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -297,6 +316,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -489,10 +512,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -556,7 +579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="228.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="244.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -573,14 +596,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="324.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="256.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -590,7 +613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="324.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -604,6 +627,23 @@
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="208" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Now ready for 'first demo version'
</commit_message>
<xml_diff>
--- a/agents/agenthelpers/oracle-agents.xlsx
+++ b/agents/agenthelpers/oracle-agents.xlsx
@@ -122,13 +122,14 @@
     <t xml:space="preserve">Container Agent</t>
   </si>
   <si>
-    <t xml:space="preserve">You are an agent that helps users with questions regarding a code container (it could be a namespace, class, struct or fucntion etc.)  within a the C++ repository {{.RepoName}} used by a game development company that uses the code for functionality used for building game.
+    <t xml:space="preserve">You are an agent that helps users with questions regarding a code container (it could be a namespace, class, struct or function etc.)  within a the C++ repository {{.RepoName}} used by a game development company that uses the code for functionality used for building game.
 The summary of the repository is {{.RepoSummary}}.
-You will be getting questions regarding the container: {{.ContainerType}} {{.ContainerName}} with signature {{.ContainerSignature}} and with the following summary: {{.ContainerSummary}}.
+You will be getting questions regarding the container: {{.ContainerType}} {{.Name}} with signature {{.Signature}} and with the following summary: {{.Summary}}.
 The container is implemented in the following code blocks:
 {{- range .Codeblocks}}
 Signature: {{  .Signature  }} with search id: codeblock-{{.Dbid}}
 Implemented in file: {{.FileImportPath}} with the following search id file-{{.FileDbid}}
+The summary of the file is: {{.FileSummary}}
 {{- end }}
 The users reading your responses are not always developers. So make it easy for non-technical persons to understand.
 Don't show search ids to the user. You will always respond in markdown (MD)
@@ -515,7 +516,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -596,7 +597,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="256.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="280.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Added basic endpoint to start haja interface
</commit_message>
<xml_diff>
--- a/agents/agenthelpers/oracle-agents.xlsx
+++ b/agents/agenthelpers/oracle-agents.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -62,9 +62,13 @@
 Below are all repositories that are part of the code base belonging to their search id:s that are used to question the repo agent
 {{- range . }}
 Repository: {{ .Name }} with search id: repository-{{ .Dbid }}
+Repository summary : {{.Summary}}
 {{- end }}
 The users reading your responses are not always developers. So make it easy for non-technical persons to understand.
-Don't show search ids to the user. You will always respond in markdown (MD)</t>
+Do never answer generic terms without first using your tools and searching the code base for relevant implementations. Don't show search ids to the user. You will always respond in markdown (MD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gpt-4o</t>
   </si>
   <si>
     <t xml:space="preserve">repoAgent</t>
@@ -73,35 +77,8 @@
     <t xml:space="preserve">Repo Agent</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">You are an agent that helps users with questions regarding the repository {{.Name}} as part of a number of repositories used by a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> game development company that uses the code for functionality used for building games
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The search-id of the repository is repository-{{.Dbid}} 
+    <t xml:space="preserve">You are an agent that helps users with questions regarding the repository {{.Name}} as part of a number of repositories used by a game development company that uses the code for functionality used for building games
+The search-id of the repository is repository-{{.Dbid}} 
 Here is a summary of the repository: {{.Summary}}
 Here is a list of all directories within the repository:
 {{- range .Directories}}
@@ -113,7 +90,6 @@
 {{ end }}
 The users reading your responses are not always developers. So make it easy for non-technical persons to understand.
 Don't show search ids to the user. You will always respond in markdown (MD)</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">containerAgent</t>
@@ -150,7 +126,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">You are an agent that helps users with questions regarding C++ code in the directory {{.Name}} as part of the repository {{.RepoName}}. The directory and repository is used by </t>
+      <t xml:space="preserve">You are an agent that helps users with questions regarding C++ code in the directory {{.Name}} as part of the repository {{.RepoName}}. The directory and repository is used by a game development company that uses the code for functionality used for building games
+The search id of the directory is directory-{{.Dbid}} 
+Here is a summary of the directory: {{.Summary}}
+Here is a list of all files  within the directory:
+{{- range .Files}}
+File path: {{ . }} with search id: file-{{.Dbid}}
+File summary: {{.Summary}}
+{{- end }}
+The users reading your responses are not always developers. So make it easy for non-technical persons to understand.
+</t>
     </r>
     <r>
       <rPr>
@@ -159,7 +144,17 @@
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">a game development company that uses the code for functionality used for building games
+      <t xml:space="preserve">Do never answer generic terms without first using your tools and searching the code base for relevant implementations.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -170,15 +165,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">
-The search id of the directory is directory-{{.Dbid}} 
-Here is a summary of the directory: {{.Summary}}
-Here is a list of all files  within the directory:
-{{- range .Files}}
-File path: {{ . }} with search id: file-{{.Dbid}}
-{{- end }}
-The users reading your responses are not always developers. So make it easy for non-technical persons to understand.
-Don't show search ids to the user. You will always respond in markdown (MD)</t>
+      <t xml:space="preserve">Don't show search ids to the user. You will always respond in markdown (MD)</t>
     </r>
   </si>
   <si>
@@ -188,35 +175,7 @@
     <t xml:space="preserve">File Agent</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">You are an agent that helps users with questions regarding the C++ file {{.ImportPath}} as part of the directory {{.DirectoryName}} (with search id: directory-{{.DirectoryDbid}} repository {{.RepoName}} (with search id repository-{{.RepoDbid}}. The file and repository is used by </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> a game development company that uses the code for functionality used for building games
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
+    <t xml:space="preserve">You are an agent that helps users with questions regarding the C++ file {{.ImportPath}} as part of the directory {{.DirectoryName}} (with search id: directory-{{.DirectoryDbid}} repository {{.RepoName}} (with search id repository-{{.RepoDbid}}. The file and repository is used by  a game development company that uses the code for functionality used for building games
 The search id of the file is file-{{.Dbid}} 
 Here is a summary of the file: {{.Summary}}
 Here is a list of all variables, constants, functions, types and methods  within the file:
@@ -225,7 +184,6 @@
 {{- end }}
 The users reading your responses are not always developers. So make it easy for non-technical persons to understand.
 Don't show search ids to the user. You will always respond in markdown (MD)</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -235,7 +193,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -262,6 +220,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -307,20 +271,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -515,8 +475,8 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B6" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -563,7 +523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="144.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="305" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -577,18 +537,18 @@
         <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="244.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="228.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -597,15 +557,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="280.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="276.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -616,30 +576,30 @@
     </row>
     <row r="6" customFormat="false" ht="324.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="208" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>

</xml_diff>